<commit_message>
Beginnings of the writeup
</commit_message>
<xml_diff>
--- a/charts.xlsx
+++ b/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27060" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>First Request</t>
   </si>
@@ -141,6 +141,30 @@
   <si>
     <t>FALL 2013 ENROLLMENTS</t>
   </si>
+  <si>
+    <t>HISTORICAL ENROLLMENT</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>F13</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
 </sst>
 </file>
 
@@ -202,7 +226,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -226,8 +250,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -241,8 +275,9 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -254,6 +289,11 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -265,6 +305,11 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9993,11 +10038,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2136955448"/>
-        <c:axId val="-2108807240"/>
+        <c:axId val="-2134434744"/>
+        <c:axId val="-2134436104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2136955448"/>
+        <c:axId val="-2134434744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -10008,12 +10053,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108807240"/>
+        <c:crossAx val="-2134436104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2108807240"/>
+        <c:axId val="-2134436104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -10031,7 +10076,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136955448"/>
+        <c:crossAx val="-2134434744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10148,11 +10193,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133605208"/>
-        <c:axId val="-2134114888"/>
+        <c:axId val="-2134557016"/>
+        <c:axId val="-2133913656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133605208"/>
+        <c:axId val="-2134557016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10161,7 +10206,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134114888"/>
+        <c:crossAx val="-2133913656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10169,7 +10214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134114888"/>
+        <c:axId val="-2133913656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20.0"/>
@@ -10187,7 +10232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133605208"/>
+        <c:crossAx val="-2134557016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="5.0"/>
@@ -10346,6 +10391,557 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Historical IntroCS</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Enrollment</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AC$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COS 109</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$AB$3:$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AC$3:$AC$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AD$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COS 126</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$AB$3:$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AD$3:$AD$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>159.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>211.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>341.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>269.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>380.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>294.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>475.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AE$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COS 217</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$AB$3:$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AE$3:$AE$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AF$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COS 226</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$AB$3:$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AF$3:$AF$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>158.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>135.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>247.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>243.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2086066936"/>
+        <c:axId val="-2086600392"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$AG$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$AB$3:$AB$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>S11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>S12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>F12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>S13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>F13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>S14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AG$3:$AG$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>347.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>547.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>596.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>632.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>747.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>701.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>840.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2086517032"/>
+        <c:axId val="-2086650520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2086066936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2086600392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2086600392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2086066936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2086650520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2086517032"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2086517032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2086650520"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -10700,11 +11296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2133666728"/>
-        <c:axId val="2133669848"/>
+        <c:axId val="-2133978408"/>
+        <c:axId val="-2134778056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133666728"/>
+        <c:axId val="-2133978408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -10713,7 +11309,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133669848"/>
+        <c:crossAx val="-2134778056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10721,7 +11317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133669848"/>
+        <c:axId val="-2134778056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300.0"/>
@@ -10739,7 +11335,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133666728"/>
+        <c:crossAx val="-2133978408"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11294,11 +11890,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2136672216"/>
-        <c:axId val="2138097512"/>
+        <c:axId val="-2134576472"/>
+        <c:axId val="-2134768936"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2136672216"/>
+        <c:axId val="-2134576472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11308,7 +11904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138097512"/>
+        <c:crossAx val="-2134768936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11318,7 +11914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2138097512"/>
+        <c:axId val="-2134768936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -11336,7 +11932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136672216"/>
+        <c:crossAx val="-2134576472"/>
         <c:crossesAt val="-1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13296,11 +13892,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134900696"/>
-        <c:axId val="-2133967704"/>
+        <c:axId val="-2134177720"/>
+        <c:axId val="-2137176424"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2134900696"/>
+        <c:axId val="-2134177720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13310,7 +13906,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133967704"/>
+        <c:crossAx val="-2137176424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13320,7 +13916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133967704"/>
+        <c:axId val="-2137176424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -13338,7 +13934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134900696"/>
+        <c:crossAx val="-2134177720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13473,11 +14069,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2106472600"/>
-        <c:axId val="-2106469592"/>
+        <c:axId val="-2138002904"/>
+        <c:axId val="-2134332168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2106472600"/>
+        <c:axId val="-2138002904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13486,7 +14082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106469592"/>
+        <c:crossAx val="-2134332168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13494,7 +14090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106469592"/>
+        <c:axId val="-2134332168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -13512,7 +14108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106472600"/>
+        <c:crossAx val="-2138002904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13624,11 +14220,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2136286648"/>
-        <c:axId val="-2136710488"/>
+        <c:axId val="2129776200"/>
+        <c:axId val="-2134505128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2136286648"/>
+        <c:axId val="2129776200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13637,7 +14233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136710488"/>
+        <c:crossAx val="-2134505128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13645,7 +14241,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2136710488"/>
+        <c:axId val="-2134505128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13662,7 +14258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2136286648"/>
+        <c:crossAx val="2129776200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13694,7 +14290,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -23246,11 +23841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142025144"/>
-        <c:axId val="-2137746792"/>
+        <c:axId val="-2134875144"/>
+        <c:axId val="-2137103416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142025144"/>
+        <c:axId val="-2134875144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23260,12 +23855,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137746792"/>
+        <c:crossAx val="-2137103416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2137746792"/>
+        <c:axId val="-2137103416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23276,14 +23871,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142025144"/>
+        <c:crossAx val="-2134875144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -23662,6 +24256,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -23987,10 +24611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1604"/>
+  <dimension ref="A1:AG1604"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Z3" activeCellId="1" sqref="X3:X6 Z3:Z6"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24005,9 +24629,10 @@
     <col min="20" max="20" width="5.6640625" style="3" customWidth="1"/>
     <col min="21" max="21" width="17.5" customWidth="1"/>
     <col min="23" max="23" width="7.5" style="3" customWidth="1"/>
+    <col min="27" max="27" width="5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -24029,8 +24654,29 @@
       <c r="X1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="AB1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="X3" s="4" t="s">
         <v>9</v>
       </c>
@@ -24041,8 +24687,28 @@
         <f>Y3/$Y$7</f>
         <v>9.9857346647646214E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="AB3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD3" s="9">
+        <v>159</v>
+      </c>
+      <c r="AE3" s="9">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>137</v>
+      </c>
+      <c r="AG3">
+        <f>SUM(AD3:AF3)</f>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
       <c r="X4" s="4" t="s">
         <v>10</v>
       </c>
@@ -24053,8 +24719,27 @@
         <f t="shared" ref="Z4:Z6" si="0">Y4/$Y$7</f>
         <v>0.41940085592011411</v>
       </c>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="AB4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="9">
+        <v>87</v>
+      </c>
+      <c r="AD4" s="9">
+        <v>211</v>
+      </c>
+      <c r="AE4" s="9">
+        <v>118</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>131</v>
+      </c>
+      <c r="AG4">
+        <f>SUM(AC4:AF4)</f>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -24113,8 +24798,28 @@
         <f t="shared" si="0"/>
         <v>0.25106990014265335</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AB5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD5" s="9">
+        <v>341</v>
+      </c>
+      <c r="AE5" s="9">
+        <v>97</v>
+      </c>
+      <c r="AF5" s="9">
+        <v>158</v>
+      </c>
+      <c r="AG5">
+        <f>SUM(AD5:AF5)</f>
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -24178,8 +24883,27 @@
         <f t="shared" si="0"/>
         <v>0.22967189728958631</v>
       </c>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="AB6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC6" s="9">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="9">
+        <v>269</v>
+      </c>
+      <c r="AE6" s="9">
+        <v>152</v>
+      </c>
+      <c r="AF6" s="9">
+        <v>135</v>
+      </c>
+      <c r="AG6">
+        <f>SUM(AC6:AF6)</f>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -24214,8 +24938,28 @@
         <f>SUM(Y3:Y6)</f>
         <v>701</v>
       </c>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="AB7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC7" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD7" s="9">
+        <v>380</v>
+      </c>
+      <c r="AE7" s="9">
+        <v>120</v>
+      </c>
+      <c r="AF7" s="9">
+        <v>247</v>
+      </c>
+      <c r="AG7">
+        <f>SUM(AD7:AF7)</f>
+        <v>747</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -24269,8 +25013,27 @@
       <c r="V8">
         <v>16.22</v>
       </c>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="AB8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>70</v>
+      </c>
+      <c r="AD8" s="9">
+        <v>294</v>
+      </c>
+      <c r="AE8" s="9">
+        <v>176</v>
+      </c>
+      <c r="AF8" s="9">
+        <v>161</v>
+      </c>
+      <c r="AG8">
+        <f>SUM(AC8:AF8)</f>
+        <v>701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -24325,8 +25088,28 @@
       <c r="V9">
         <v>14.38</v>
       </c>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="AB9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC9" s="9" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AD9" s="9">
+        <v>475</v>
+      </c>
+      <c r="AE9" s="9">
+        <v>122</v>
+      </c>
+      <c r="AF9" s="9">
+        <v>243</v>
+      </c>
+      <c r="AG9">
+        <f>SUM(AD9:AF9)</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -24382,7 +25165,7 @@
         <v>16.57</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:33">
       <c r="D11" s="4" t="s">
         <v>17</v>
       </c>
@@ -24431,7 +25214,7 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:33">
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
@@ -24474,7 +25257,7 @@
         <v>34.049999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:33">
       <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
@@ -24517,7 +25300,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:33">
       <c r="D14" s="4" t="s">
         <v>20</v>
       </c>
@@ -24556,7 +25339,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:33">
       <c r="L15">
         <v>7</v>
       </c>
@@ -24570,7 +25353,7 @@
         <v>0.15872184389732799</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:33">
       <c r="L16">
         <v>8</v>
       </c>
@@ -39262,8 +40045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>